<commit_message>
Praktikum 1 – Membuat RESTful API Register
</commit_message>
<xml_diff>
--- a/public/template_user.xlsx
+++ b/public/template_user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1866635-E55D-4BE9-B4E8-3FEBD7EA108E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5E8407-64DC-4DDC-8D07-04402325CD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D754B2BC-5FA2-447A-8CE0-378589DF70ED}"/>
   </bookViews>
@@ -38,22 +38,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>nama</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Direktur</t>
+  </si>
+  <si>
+    <t>Om Direktur</t>
+  </si>
+  <si>
     <t>level_id</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>nama</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Direktur</t>
-  </si>
-  <si>
-    <t>Om Direktur</t>
   </si>
 </sst>
 </file>
@@ -437,34 +437,34 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2">
         <v>12345</v>

</xml_diff>